<commit_message>
update Team Report :Sprint1 review, Sprint 2 plan, Burn down
</commit_message>
<xml_diff>
--- a/docs/TeamHogwartsReport.xlsx
+++ b/docs/TeamHogwartsReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huying/Dropbox-yhu@stevens/Dropbox/My Dropbox Move/0_SSW-555/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huying/GitHub/ssw555tmHogwarts2020Spring/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA9AF16-5A01-DE47-BD40-F753BF809A14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC17ED6-FE5A-1F41-8AAB-96187BFD79E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="620" windowWidth="25600" windowHeight="15480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="15540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,15 +37,34 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="271">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -150,10 +170,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>hm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Story ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -166,10 +182,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -189,15 +201,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
   <si>
@@ -624,15 +627,6 @@
     <t>Source File</t>
   </si>
   <si>
-    <t>gedcom.py</t>
-  </si>
-  <si>
-    <t>us03_birth_b4_death</t>
-  </si>
-  <si>
-    <t>33-36</t>
-  </si>
-  <si>
     <t>Test File</t>
   </si>
   <si>
@@ -648,15 +642,6 @@
     <t>Test lines</t>
   </si>
   <si>
-    <t>test_us03</t>
-  </si>
-  <si>
-    <t>15-23</t>
-  </si>
-  <si>
-    <t>test03.py</t>
-  </si>
-  <si>
     <t>yz</t>
   </si>
   <si>
@@ -723,9 +708,6 @@
     <t>zy</t>
   </si>
   <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
     <t>Estimation</t>
   </si>
   <si>
@@ -748,6 +730,183 @@
   </si>
   <si>
     <t>Epimetheus12</t>
+  </si>
+  <si>
+    <t>Collaboration Model:</t>
+  </si>
+  <si>
+    <t>Collaborator</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>works as the production environment, which stores codes and files of completed sprints.</t>
+  </si>
+  <si>
+    <t>Devolop</t>
+  </si>
+  <si>
+    <t>works as the developing environment, which stores codes and files of the current working sprint. When a sprint completed, this branch will be merged into Master Branch, operated by Yu Zhou only.</t>
+  </si>
+  <si>
+    <t>Story Velocity</t>
+  </si>
+  <si>
+    <t>Unify name rule to avoid conflicts</t>
+  </si>
+  <si>
+    <t>Coding without comments</t>
+  </si>
+  <si>
+    <t>Communicate in time</t>
+  </si>
+  <si>
+    <t>The main file should be revised ASAP if needs arises, or it'll occur a lot of rework</t>
+  </si>
+  <si>
+    <t>us02.py</t>
+  </si>
+  <si>
+    <t>us03.py</t>
+  </si>
+  <si>
+    <t>us04.py</t>
+  </si>
+  <si>
+    <t>us05.py</t>
+  </si>
+  <si>
+    <t>us07.py</t>
+  </si>
+  <si>
+    <t>us01.py</t>
+  </si>
+  <si>
+    <t>us08.py</t>
+  </si>
+  <si>
+    <t>us09.py</t>
+  </si>
+  <si>
+    <t>us02_test.py</t>
+  </si>
+  <si>
+    <t>us03_test.py</t>
+  </si>
+  <si>
+    <t>us04_test.py</t>
+  </si>
+  <si>
+    <t>us05_test.py</t>
+  </si>
+  <si>
+    <t>us01_test.py</t>
+  </si>
+  <si>
+    <t>us07_test.py</t>
+  </si>
+  <si>
+    <t>us08_test.py</t>
+  </si>
+  <si>
+    <t>us09_test.py</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>us01_current_date_check</t>
+  </si>
+  <si>
+    <t>us02_birth_before_marriage</t>
+  </si>
+  <si>
+    <t>us03_birth_before_death</t>
+  </si>
+  <si>
+    <t>us04_marriage_before_divorce</t>
+  </si>
+  <si>
+    <t>us05_marriage_before_death</t>
+  </si>
+  <si>
+    <t>us07_not_olderthan150</t>
+  </si>
+  <si>
+    <t>us08_birth_before_marriage</t>
+  </si>
+  <si>
+    <t>us09_birth_after_death</t>
+  </si>
+  <si>
+    <t>6-41</t>
+  </si>
+  <si>
+    <t>Testcurrent_date_check</t>
+  </si>
+  <si>
+    <t>10-23</t>
+  </si>
+  <si>
+    <t>10-32</t>
+  </si>
+  <si>
+    <t>Testbirth_before_marriage</t>
+  </si>
+  <si>
+    <t>10-22</t>
+  </si>
+  <si>
+    <t>6-23</t>
+  </si>
+  <si>
+    <t>US04_TestCase</t>
+  </si>
+  <si>
+    <t>11-25</t>
+  </si>
+  <si>
+    <t>6-30</t>
+  </si>
+  <si>
+    <t>US05_TestCase</t>
+  </si>
+  <si>
+    <t>11-23</t>
+  </si>
+  <si>
+    <t>6-25</t>
+  </si>
+  <si>
+    <t>10-21</t>
+  </si>
+  <si>
+    <t>5-18</t>
+  </si>
+  <si>
+    <t>US08_TestCase</t>
+  </si>
+  <si>
+    <t>11-24</t>
+  </si>
+  <si>
+    <t>5-19</t>
+  </si>
+  <si>
+    <t>US09_TestCase</t>
+  </si>
+  <si>
+    <t>Asserting GED data opptionally, it may probaberly affect previous us test. Instead, we shall always add new GED data at the end of the GED file.</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>(expected)</t>
+  </si>
+  <si>
+    <t>Doing</t>
   </si>
 </sst>
 </file>
@@ -805,7 +964,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -820,24 +979,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -918,6 +1071,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -987,7 +1155,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1008,28 +1176,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1037,47 +1192,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1088,35 +1216,107 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1361,19 +1561,37 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:f>Burndown!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>42406</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42427</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42483</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>Burndown!$C$2:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1397,7 +1615,7 @@
         <c:axId val="1158123744"/>
         <c:axId val="1158126064"/>
       </c:lineChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1158123744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -1411,10 +1629,9 @@
         <c:crossAx val="1158126064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="1158126064"/>
         <c:scaling>
@@ -1423,7 +1640,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1904,13 +2121,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>948267</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>160867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>397934</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
@@ -2261,117 +2478,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="E1" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D8" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="D8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>204</v>
-      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D9" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D10" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+    </row>
+    <row r="11" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D11" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" s="66" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
     <sortCondition ref="C2:C4"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{491585F5-1070-FA43-806C-9162A05F1980}"/>
@@ -2386,39 +2635,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14" style="22" customWidth="1"/>
-    <col min="3" max="3" width="36" style="22" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="60" customWidth="1"/>
+    <col min="2" max="2" width="14" style="17" customWidth="1"/>
+    <col min="3" max="3" width="36" style="17" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="53" t="s">
+    <row r="1" spans="1:9" s="16" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="52" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="52" t="s">
+      <c r="E1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="45" t="s">
-        <v>29</v>
-      </c>
       <c r="F1" s="13" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -2428,168 +2677,466 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="str">
-        <f>Sprint1!A5</f>
+      <c r="B2" s="17" t="str">
+        <f>Sprint1!A3</f>
         <v>US02</v>
       </c>
-      <c r="C2" s="22" t="str">
-        <f>Sprint1!B5</f>
+      <c r="C2" s="17" t="str">
+        <f>Sprint1!B3</f>
         <v>Birth before marriage</v>
       </c>
-      <c r="D2" s="22" t="str">
-        <f>Sprint1!C5</f>
+      <c r="D2" s="17" t="str">
+        <f>Sprint1!C3</f>
         <v>hy</v>
       </c>
-      <c r="E2" s="60" t="str">
-        <f>Sprint1!D5</f>
-        <v>To do</v>
+      <c r="E2" s="36" t="str">
+        <f>Sprint1!D3</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="str">
-        <f>Sprint1!A6</f>
+      <c r="B3" s="17" t="str">
+        <f>Sprint1!A4</f>
         <v>US03</v>
       </c>
-      <c r="C3" s="22" t="str">
-        <f>Sprint1!B6</f>
+      <c r="C3" s="17" t="str">
+        <f>Sprint1!B4</f>
         <v>Birth before death</v>
       </c>
-      <c r="D3" s="22" t="str">
-        <f>Sprint1!C6</f>
+      <c r="D3" s="17" t="str">
+        <f>Sprint1!C4</f>
         <v>hy</v>
       </c>
-      <c r="E3" s="60" t="str">
-        <f>Sprint1!D6</f>
-        <v>To do</v>
+      <c r="E3" s="36" t="str">
+        <f>Sprint1!D4</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="22" t="str">
-        <f>Sprint1!A7</f>
+      <c r="B4" s="17" t="str">
+        <f>Sprint1!A5</f>
         <v>US04</v>
       </c>
-      <c r="C4" s="22" t="str">
-        <f>Sprint1!B7</f>
+      <c r="C4" s="17" t="str">
+        <f>Sprint1!B5</f>
         <v>Marriage before divorce</v>
       </c>
-      <c r="D4" s="22" t="str">
-        <f>Sprint1!C7</f>
+      <c r="D4" s="17" t="str">
+        <f>Sprint1!C5</f>
         <v>zy</v>
       </c>
-      <c r="E4" s="60" t="str">
-        <f>Sprint1!D7</f>
-        <v>To do</v>
+      <c r="E4" s="36" t="str">
+        <f>Sprint1!D5</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="22" t="str">
-        <f>Sprint1!A8</f>
+      <c r="B5" s="17" t="str">
+        <f>Sprint1!A6</f>
         <v>US05</v>
       </c>
-      <c r="C5" s="22" t="str">
-        <f>Sprint1!B8</f>
+      <c r="C5" s="17" t="str">
+        <f>Sprint1!B6</f>
         <v>Marriage before death</v>
       </c>
-      <c r="D5" s="22" t="str">
-        <f>Sprint1!C8</f>
+      <c r="D5" s="17" t="str">
+        <f>Sprint1!C6</f>
         <v>zy</v>
       </c>
-      <c r="E5" s="60" t="str">
-        <f>Sprint1!D8</f>
-        <v>To do</v>
+      <c r="E5" s="36" t="str">
+        <f>Sprint1!D6</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="22" t="str">
-        <f>Sprint1!A9</f>
+      <c r="B6" s="17" t="str">
+        <f>Sprint1!A7</f>
         <v>US01</v>
       </c>
-      <c r="C6" s="22" t="str">
-        <f>Sprint1!B9</f>
+      <c r="C6" s="17" t="str">
+        <f>Sprint1!B7</f>
         <v>Dates before current date</v>
       </c>
-      <c r="D6" s="22" t="str">
-        <f>Sprint1!C9</f>
+      <c r="D6" s="17" t="str">
+        <f>Sprint1!C7</f>
         <v>hw</v>
       </c>
-      <c r="E6" s="60" t="str">
-        <f>Sprint1!D9</f>
-        <v>To do</v>
+      <c r="E6" s="36" t="str">
+        <f>Sprint1!D7</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="22" t="str">
-        <f>Sprint1!A10</f>
+      <c r="B7" s="17" t="str">
+        <f>Sprint1!A8</f>
         <v>US07</v>
       </c>
-      <c r="C7" s="22" t="str">
-        <f>Sprint1!B10</f>
+      <c r="C7" s="17" t="str">
+        <f>Sprint1!B8</f>
         <v>Less then 150 years old</v>
       </c>
-      <c r="D7" s="22" t="str">
-        <f>Sprint1!C10</f>
+      <c r="D7" s="17" t="str">
+        <f>Sprint1!C8</f>
         <v>hw</v>
       </c>
-      <c r="E7" s="60" t="str">
-        <f>Sprint1!D10</f>
-        <v>To do</v>
+      <c r="E7" s="36" t="str">
+        <f>Sprint1!D8</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="22" t="str">
-        <f>Sprint1!A11</f>
+      <c r="B8" s="17" t="str">
+        <f>Sprint1!A9</f>
         <v>US08</v>
       </c>
-      <c r="C8" s="22" t="str">
-        <f>Sprint1!B11</f>
+      <c r="C8" s="17" t="str">
+        <f>Sprint1!B9</f>
         <v>Birth before marriage of parents</v>
       </c>
-      <c r="D8" s="22" t="str">
-        <f>Sprint1!C11</f>
+      <c r="D8" s="17" t="str">
+        <f>Sprint1!C9</f>
         <v>fl</v>
       </c>
-      <c r="E8" s="60" t="str">
-        <f>Sprint1!D11</f>
-        <v>To do</v>
+      <c r="E8" s="36" t="str">
+        <f>Sprint1!D9</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="22" t="str">
-        <f>Sprint1!A12</f>
+      <c r="B9" s="17" t="str">
+        <f>Sprint1!A10</f>
         <v>US09</v>
       </c>
-      <c r="C9" s="22" t="str">
-        <f>Sprint1!B12</f>
+      <c r="C9" s="17" t="str">
+        <f>Sprint1!B10</f>
         <v>Birth before death of parents</v>
       </c>
-      <c r="D9" s="22" t="str">
-        <f>Sprint1!C12</f>
+      <c r="D9" s="17" t="str">
+        <f>Sprint1!C10</f>
         <v>fl</v>
       </c>
-      <c r="E9" s="60" t="str">
-        <f>Sprint1!D12</f>
+      <c r="E9" s="36" t="str">
+        <f>Sprint1!D10</f>
+        <v>Done</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="17" t="str" cm="1">
+        <f t="array" ref="B10:E17">Sprint2!A3:D10</f>
+        <v>US06</v>
+      </c>
+      <c r="C10" s="17" t="str">
+        <v>Divorce before death</v>
+      </c>
+      <c r="D10" s="17" t="str">
+        <v>yh</v>
+      </c>
+      <c r="E10" s="36" t="str">
+        <v>Doing</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="17" t="str">
+        <v>US10</v>
+      </c>
+      <c r="C11" s="17" t="str">
+        <v>Marriage after 14</v>
+      </c>
+      <c r="D11" s="17" t="str">
+        <v>yz</v>
+      </c>
+      <c r="E11" s="36" t="str">
         <v>To do</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="17" t="str">
+        <v>US12</v>
+      </c>
+      <c r="C12" s="17" t="str">
+        <v>Parents not too old</v>
+      </c>
+      <c r="D12" s="17" t="str">
+        <v>yh</v>
+      </c>
+      <c r="E12" s="36" t="str">
+        <v>Doing</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="17" t="str">
+        <v>US11</v>
+      </c>
+      <c r="C13" s="17" t="str">
+        <v>No bigamy</v>
+      </c>
+      <c r="D13" s="17" t="str">
+        <v>yz</v>
+      </c>
+      <c r="E13" s="36" t="str">
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="17" t="str">
+        <v>US17</v>
+      </c>
+      <c r="C14" s="17" t="str">
+        <v>No marriages to children</v>
+      </c>
+      <c r="D14" s="17" t="str">
+        <v>hw</v>
+      </c>
+      <c r="E14" s="36" t="str">
+        <v>Doing</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="17" t="str">
+        <v>US18</v>
+      </c>
+      <c r="C15" s="17" t="str">
+        <v>Siblings should not marry</v>
+      </c>
+      <c r="D15" s="17" t="str">
+        <v>hw</v>
+      </c>
+      <c r="E15" s="36" t="str">
+        <v>Doing</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="17" t="str">
+        <v>US15</v>
+      </c>
+      <c r="C16" s="17" t="str">
+        <v>Fewer than 15 siblings</v>
+      </c>
+      <c r="D16" s="17" t="str">
+        <v>fl</v>
+      </c>
+      <c r="E16" s="36" t="str">
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="17" t="str">
+        <v>US16</v>
+      </c>
+      <c r="C17" s="17" t="str">
+        <v>Male last names</v>
+      </c>
+      <c r="D17" s="17" t="str">
+        <v>fl</v>
+      </c>
+      <c r="E17" s="36" t="str">
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B18" s="17" t="str" cm="1">
+        <f t="array" ref="B18:C37">Stories!A21:B40</f>
+        <v>US20</v>
+      </c>
+      <c r="C18" s="17" t="str">
+        <v>Aunts and uncles</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B19" s="17" t="str">
+        <v>US21</v>
+      </c>
+      <c r="C19" s="17" t="str">
+        <v>Correct gender for role</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B20" s="17" t="str">
+        <v>US22</v>
+      </c>
+      <c r="C20" s="17" t="str">
+        <v>Unique IDs</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B21" s="17" t="str">
+        <v>US23</v>
+      </c>
+      <c r="C21" s="17" t="str">
+        <v>Unique name and birth date</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B22" s="17" t="str">
+        <v>US24</v>
+      </c>
+      <c r="C22" s="17" t="str">
+        <v>Unique families by spouses</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B23" s="17" t="str">
+        <v>US25</v>
+      </c>
+      <c r="C23" s="17" t="str">
+        <v>Unique first names in families</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B24" s="17" t="str">
+        <v>US26</v>
+      </c>
+      <c r="C24" s="17" t="str">
+        <v>Corresponding entries</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B25" s="17" t="str">
+        <v>US27</v>
+      </c>
+      <c r="C25" s="17" t="str">
+        <v>Include individual ages</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B26" s="17" t="str">
+        <v>US28</v>
+      </c>
+      <c r="C26" s="17" t="str">
+        <v>Order siblings by age</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B27" s="17" t="str">
+        <v>US29</v>
+      </c>
+      <c r="C27" s="17" t="str">
+        <v>List deceased</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B28" s="17" t="str">
+        <v>US30</v>
+      </c>
+      <c r="C28" s="17" t="str">
+        <v>List living married</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B29" s="17" t="str">
+        <v>US31</v>
+      </c>
+      <c r="C29" s="17" t="str">
+        <v>List living single</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B30" s="17" t="str">
+        <v>US32</v>
+      </c>
+      <c r="C30" s="17" t="str">
+        <v>List multiple births</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B31" s="17" t="str">
+        <v>US33</v>
+      </c>
+      <c r="C31" s="17" t="str">
+        <v>List orphans</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B32" s="17" t="str">
+        <v>US34</v>
+      </c>
+      <c r="C32" s="17" t="str">
+        <v>List large age differences</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B33" s="17" t="str">
+        <v>US35</v>
+      </c>
+      <c r="C33" s="17" t="str">
+        <v>List recent births</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B34" s="17" t="str">
+        <v>US36</v>
+      </c>
+      <c r="C34" s="17" t="str">
+        <v>List recent deaths</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B35" s="17" t="str">
+        <v>US37</v>
+      </c>
+      <c r="C35" s="17" t="str">
+        <v>List recent survivors</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B36" s="17" t="str">
+        <v>US38</v>
+      </c>
+      <c r="C36" s="17" t="str">
+        <v>List upcoming birthdays</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B37" s="17" t="str">
+        <v>US39</v>
+      </c>
+      <c r="C37" s="17" t="str">
+        <v>List upcoming anniversaries</v>
       </c>
     </row>
   </sheetData>
@@ -2603,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2619,37 +3166,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>0</v>
@@ -2672,7 +3219,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B15" s="8">
         <v>41065</v>
@@ -2688,7 +3235,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B16" s="8">
         <v>41078</v>
@@ -2713,7 +3260,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B17" s="8">
         <v>41092</v>
@@ -2738,7 +3285,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B18" s="8">
         <v>41106</v>
@@ -2763,7 +3310,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B19" s="8">
         <v>41120</v>
@@ -2795,41 +3342,127 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="60">
+        <v>42406</v>
+      </c>
+      <c r="C2" s="62">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="63">
+        <v>0</v>
+      </c>
+      <c r="F2" s="63"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42427</v>
+      </c>
+      <c r="C3" s="62">
+        <f>32-8</f>
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="63">
+        <f>SUM(Sprint1!G3:G10)</f>
+        <v>196</v>
+      </c>
+      <c r="F3" s="63">
+        <f>SUM(Sprint1!H3:H10)</f>
+        <v>460</v>
+      </c>
+      <c r="G3" s="7">
+        <f>(E3-E2)/F3*60</f>
+        <v>25.565217391304348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="62"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="62"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="62"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" s="75">
+        <v>42483</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="C8" s="61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2841,402 +3474,568 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.83203125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="24" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="18" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.6640625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="13" style="51" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="56" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="20" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:16" s="16" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
-    </row>
-    <row r="2" spans="1:16" s="20" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="32" t="s">
+      <c r="E1" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" s="69"/>
+    </row>
+    <row r="2" spans="1:16" s="16" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="K2" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="O2" s="35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="21" t="s">
+    </row>
+    <row r="3" spans="1:16" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="17">
+        <v>10</v>
+      </c>
+      <c r="F3">
         <v>30</v>
       </c>
-      <c r="E3" s="21">
-        <v>150</v>
-      </c>
-      <c r="F3" s="16">
+      <c r="G3" s="17">
+        <v>30</v>
+      </c>
+      <c r="H3" s="39">
         <v>60</v>
       </c>
-      <c r="G3" s="21">
-        <v>120</v>
-      </c>
-      <c r="H3" s="16">
-        <v>90</v>
-      </c>
-      <c r="I3" s="17">
-        <v>40444</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="M3" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>215</v>
+      <c r="I3" s="4">
+        <v>42423</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>248</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="O3" s="57" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A4" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E4" s="17">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4">
+        <v>42423</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="L4" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="O4" s="57" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A5" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E5" s="22">
-        <v>10</v>
+      <c r="A5" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" s="17">
+        <v>15</v>
       </c>
       <c r="F5">
         <v>30</v>
       </c>
+      <c r="G5" s="17">
+        <v>23</v>
+      </c>
+      <c r="H5" s="39">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4">
+        <v>42425</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="L5" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="O5" s="57" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A6" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>212</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E6" s="22">
-        <v>10</v>
+      <c r="A6" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="17">
+        <v>15</v>
       </c>
       <c r="F6">
         <v>30</v>
       </c>
+      <c r="G6" s="17">
+        <v>30</v>
+      </c>
+      <c r="H6" s="39">
+        <v>45</v>
+      </c>
+      <c r="I6" s="4">
+        <v>42425</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="L6" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="O6" s="57" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E7" s="17">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" s="17">
+        <v>41</v>
+      </c>
+      <c r="H7" s="39">
+        <v>180</v>
+      </c>
+      <c r="I7" s="4">
+        <v>42417</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="L7" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="O7" s="57" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A8" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E8" s="17">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8" s="17">
+        <v>25</v>
+      </c>
+      <c r="H8" s="39">
+        <v>10</v>
+      </c>
+      <c r="I8" s="4">
+        <v>42417</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="L8" s="52" t="s">
+        <v>260</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="O8" s="57" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A9" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E9" s="17">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9" s="17">
+        <v>13</v>
+      </c>
+      <c r="H9" s="39">
+        <v>40</v>
+      </c>
+      <c r="I9" s="4">
+        <v>42425</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="L9" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="O9" s="57" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A10" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B10" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="D7" s="36" t="s">
+      <c r="C10" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" s="17">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10" s="17">
+        <v>14</v>
+      </c>
+      <c r="H10" s="39">
+        <v>20</v>
+      </c>
+      <c r="I10" s="4">
+        <v>42425</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="L10" s="52" t="s">
+        <v>265</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O10" s="57" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="B13" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="B14" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="41">
+        <v>1</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="47"/>
+    </row>
+    <row r="16" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="41">
+        <v>2</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="47"/>
+    </row>
+    <row r="17" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="41">
+        <v>3</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="14" x14ac:dyDescent="0.15">
+      <c r="B18" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="43" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="41">
+        <v>1</v>
+      </c>
+      <c r="B19" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="E7" s="22">
-        <v>15</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A8" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E8" s="22">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A9" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E9" s="22">
-        <v>15</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="31"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A10" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E10" s="22">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A11" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E11" s="22">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="A12" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="E12" s="22">
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="B15" s="25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
-      <c r="B16" s="25"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="B17" s="25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="28" x14ac:dyDescent="0.15">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="28" x14ac:dyDescent="0.15">
-      <c r="A19" s="37"/>
-      <c r="B19" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="14" x14ac:dyDescent="0.15">
-      <c r="B21" s="25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="28" x14ac:dyDescent="0.15">
-      <c r="A22" s="37"/>
-      <c r="B22" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="19" t="s">
-        <v>215</v>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="47"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A20" s="41">
+        <v>2</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3258,16 +4057,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
@@ -3284,78 +4083,237 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="E1" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" s="69"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="32" t="s">
+      <c r="A2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="K2" s="33" t="s">
+    </row>
+    <row r="3" spans="1:15" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A6" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6">
+        <v>60</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A7" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="L2" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="O2" s="35" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
+      <c r="D9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A10" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="J1:L1"/>
@@ -3390,75 +4348,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="E1" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" s="69"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="32" t="s">
+      <c r="A2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="O2" s="35" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
@@ -3496,75 +4454,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="54" t="s">
-        <v>216</v>
-      </c>
-      <c r="F1" s="55"/>
-      <c r="G1" s="54" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="E1" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" s="69"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="32" t="s">
+      <c r="A2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>181</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="O2" s="35" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
@@ -3588,516 +4546,531 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="47"/>
-    <col min="2" max="2" width="28.1640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="49" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="47"/>
+    <col min="1" max="1" width="10.83203125" style="29"/>
+    <col min="2" max="2" width="28.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="31" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:4" s="16" customFormat="1" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="35" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A3" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A4" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A5" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A6" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B6" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C6" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A7" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="35" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="48" t="s">
+      <c r="C7" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="46" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A3" s="46" t="s">
+      <c r="D7" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+      <c r="A8" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B8" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="D8" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A9" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A10" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+      <c r="A11" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A12" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="46" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A4" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="48" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+      <c r="A13" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+      <c r="A14" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A15" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="46" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A5" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="48" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A16" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="46" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A6" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="48" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A17" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="46" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A7" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="48" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A18" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A19" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
-      <c r="A8" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A9" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A10" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
-      <c r="A11" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A12" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="48" t="s">
+      <c r="D19" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A20" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
-      <c r="A13" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="48" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
-      <c r="A14" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="47" t="s">
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A21" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A15" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="47" t="s">
+      <c r="C21" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A22" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A23" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A24" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+      <c r="A25" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A26" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
+      <c r="A27" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A28" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A29" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A16" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A17" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
-      <c r="A18" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
-      <c r="A19" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
-      <c r="A20" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A21" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="48" t="s">
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A30" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A22" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A23" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A24" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="48" t="s">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+      <c r="A31" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
-      <c r="A25" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="48" t="s">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
+      <c r="A32" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A26" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="B26" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="48" t="s">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A33" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
-      <c r="A27" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="B27" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A28" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="B28" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="C28" s="48" t="s">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A34" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A29" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="48" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
-      <c r="A30" s="47" t="s">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A35" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B35" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A36" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="48" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
-      <c r="A31" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B31" s="47" t="s">
+      <c r="C36" s="30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A37" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A32" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="47" t="s">
+      <c r="C37" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A38" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
-      <c r="A33" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="47" t="s">
+      <c r="C38" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A39" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A34" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="B34" s="47" t="s">
+      <c r="C39" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A40" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
-      <c r="A35" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="B35" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="48" t="s">
+      <c r="C40" s="30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A36" s="47" t="s">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A41" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B41" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C41" s="30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A42" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A37" s="47" t="s">
-        <v>152</v>
-      </c>
-      <c r="B37" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="48" t="s">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A43" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="30" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A38" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="B38" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A39" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="B39" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A40" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="B40" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="48" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A41" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="B41" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A42" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="B42" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
-      <c r="A43" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="B43" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C43" s="48" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sprint 3 plan
</commit_message>
<xml_diff>
--- a/docs/TeamHogwartsReport.xlsx
+++ b/docs/TeamHogwartsReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeyiszy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huying/GitHub/ssw555tmHogwarts2020Spring/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2D82C87-2112-6349-BBF1-5F8E49993672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DBE56-557F-0A47-BD87-D10043993CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="15540" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25560" windowHeight="15540" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="293">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -860,9 +860,6 @@
     <t>Asserting GED data opptionally, it may probaberly affect previous us test. Instead, we shall always add new GED data at the end of the GED file.</t>
   </si>
   <si>
-    <t>Doing</t>
-  </si>
-  <si>
     <t>1-23</t>
   </si>
   <si>
@@ -972,6 +969,18 @@
   <si>
     <t>11-21</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Keep refactorying if needs arise</t>
+  </si>
+  <si>
+    <t>Try Mock from Sprint 3 for test code</t>
+  </si>
+  <si>
+    <t>duplication</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -979,8 +988,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1233,18 +1242,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1276,7 +1285,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,7 +1327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1360,13 +1369,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1397,74 +1406,101 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="65" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1482,7 +1518,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1629,7 +1665,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2736,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2974,7 +3010,7 @@
         <v>yz</v>
       </c>
       <c r="E11" s="36" t="str">
-        <v>To do</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3008,7 +3044,7 @@
         <v>yz</v>
       </c>
       <c r="E13" s="36" t="str">
-        <v>To do</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3025,7 +3061,7 @@
         <v>hw</v>
       </c>
       <c r="E14" s="36" t="str">
-        <v>Doing</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3042,7 +3078,7 @@
         <v>hw</v>
       </c>
       <c r="E15" s="36" t="str">
-        <v>Doing</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3059,7 +3095,7 @@
         <v>fl</v>
       </c>
       <c r="E16" s="36" t="str">
-        <v>To do</v>
+        <v>Done</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3076,169 +3112,210 @@
         <v>fl</v>
       </c>
       <c r="E17" s="36" t="str">
+        <v>Done</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="29">
+        <v>3</v>
+      </c>
+      <c r="B18" s="29" t="str">
+        <f>Sprint3!A3</f>
+        <v>US13</v>
+      </c>
+      <c r="C18" s="29" t="str">
+        <f>Sprint3!B3</f>
+        <v>Siblings spacing</v>
+      </c>
+      <c r="D18" s="29" t="str">
+        <f>Sprint3!C3</f>
+        <v>yz</v>
+      </c>
+      <c r="E18" s="29" t="str">
+        <f>Sprint3!D3</f>
         <v>To do</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="B18" s="17" t="str" cm="1">
-        <f t="array" ref="B18:C37">Stories!A21:B40</f>
+    <row r="19" spans="1:5">
+      <c r="A19" s="29">
+        <v>3</v>
+      </c>
+      <c r="B19" s="29" t="str">
+        <f>Sprint3!A4</f>
+        <v>US14</v>
+      </c>
+      <c r="C19" s="29" t="str">
+        <f>Sprint3!B4</f>
+        <v>Multiple births &lt;= 5</v>
+      </c>
+      <c r="D19" s="29" t="str">
+        <f>Sprint3!C4</f>
+        <v>yz</v>
+      </c>
+      <c r="E19" s="29" t="str">
+        <f>Sprint3!D4</f>
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="29">
+        <v>3</v>
+      </c>
+      <c r="B20" s="29" t="str">
+        <f>Sprint3!A5</f>
+        <v>US19</v>
+      </c>
+      <c r="C20" s="29" t="str">
+        <f>Sprint3!B5</f>
+        <v>First cousins should not marry</v>
+      </c>
+      <c r="D20" s="29" t="str">
+        <f>Sprint3!C5</f>
+        <v>fl</v>
+      </c>
+      <c r="E20" s="29" t="str">
+        <f>Sprint3!D5</f>
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="29">
+        <v>3</v>
+      </c>
+      <c r="B21" s="29" t="str">
+        <f>Sprint3!A6</f>
         <v>US20</v>
       </c>
-      <c r="C18" s="17" t="str">
+      <c r="C21" s="29" t="str">
+        <f>Sprint3!B6</f>
         <v>Aunts and uncles</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" s="17" t="str">
+      <c r="D21" s="29" t="str">
+        <f>Sprint3!C6</f>
+        <v>fl</v>
+      </c>
+      <c r="E21" s="29" t="str">
+        <f>Sprint3!D6</f>
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="29">
+        <v>3</v>
+      </c>
+      <c r="B22" s="29" t="str">
+        <f>Sprint3!A7</f>
         <v>US21</v>
       </c>
-      <c r="C19" s="17" t="str">
+      <c r="C22" s="29" t="str">
+        <f>Sprint3!B7</f>
         <v>Correct gender for role</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" s="17" t="str">
+      <c r="D22" s="29" t="str">
+        <f>Sprint3!C7</f>
+        <v>hw</v>
+      </c>
+      <c r="E22" s="29" t="str">
+        <f>Sprint3!D7</f>
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="29">
+        <v>3</v>
+      </c>
+      <c r="B23" s="29" t="str">
+        <f>Sprint3!A8</f>
         <v>US22</v>
       </c>
-      <c r="C20" s="17" t="str">
+      <c r="C23" s="29" t="str">
+        <f>Sprint3!B8</f>
         <v>Unique IDs</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" s="17" t="str">
+      <c r="D23" s="29" t="str">
+        <f>Sprint3!C8</f>
+        <v>hw</v>
+      </c>
+      <c r="E23" s="29" t="str">
+        <f>Sprint3!D8</f>
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="29">
+        <v>3</v>
+      </c>
+      <c r="B24" s="29" t="str">
+        <f>Sprint3!A9</f>
         <v>US23</v>
       </c>
-      <c r="C21" s="17" t="str">
+      <c r="C24" s="29" t="str">
+        <f>Sprint3!B9</f>
         <v>Unique name and birth date</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" s="17" t="str">
+      <c r="D24" s="29" t="str">
+        <f>Sprint3!C9</f>
+        <v>yh</v>
+      </c>
+      <c r="E24" s="29" t="str">
+        <f>Sprint3!D9</f>
+        <v>To do</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="29">
+        <v>3</v>
+      </c>
+      <c r="B25" s="29" t="str">
+        <f>Sprint3!A10</f>
         <v>US24</v>
       </c>
-      <c r="C22" s="17" t="str">
+      <c r="C25" s="29" t="str">
+        <f>Sprint3!B10</f>
         <v>Unique families by spouses</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="17" t="str">
-        <v>US25</v>
-      </c>
-      <c r="C23" s="17" t="str">
-        <v>Unique first names in families</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" s="17" t="str">
-        <v>US26</v>
-      </c>
-      <c r="C24" s="17" t="str">
-        <v>Corresponding entries</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" s="17" t="str">
-        <v>US27</v>
-      </c>
-      <c r="C25" s="17" t="str">
-        <v>Include individual ages</v>
+      <c r="D25" s="29" t="str">
+        <f>Sprint3!C10</f>
+        <v>yh</v>
+      </c>
+      <c r="E25" s="29" t="str">
+        <f>Sprint3!D10</f>
+        <v>To do</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="17" t="str">
-        <v>US28</v>
-      </c>
-      <c r="C26" s="17" t="str">
-        <v>Order siblings by age</v>
-      </c>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="B27" s="17" t="str">
-        <v>US29</v>
-      </c>
-      <c r="C27" s="17" t="str">
-        <v>List deceased</v>
-      </c>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="17" t="str">
-        <v>US30</v>
-      </c>
-      <c r="C28" s="17" t="str">
-        <v>List living married</v>
-      </c>
+      <c r="A28" s="29"/>
+      <c r="B28" s="64"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="B29" s="17" t="str">
-        <v>US31</v>
-      </c>
-      <c r="C29" s="17" t="str">
-        <v>List living single</v>
-      </c>
+      <c r="A29" s="29"/>
+      <c r="B29" s="64"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="17" t="str">
-        <v>US32</v>
-      </c>
-      <c r="C30" s="17" t="str">
-        <v>List multiple births</v>
-      </c>
+      <c r="A30" s="29"/>
+      <c r="B30" s="64"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" s="17" t="str">
-        <v>US33</v>
-      </c>
-      <c r="C31" s="17" t="str">
-        <v>List orphans</v>
-      </c>
+      <c r="A31" s="29"/>
+      <c r="B31" s="64"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="17" t="str">
-        <v>US34</v>
-      </c>
-      <c r="C32" s="17" t="str">
-        <v>List large age differences</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="17" t="str">
-        <v>US35</v>
-      </c>
-      <c r="C33" s="17" t="str">
-        <v>List recent births</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="17" t="str">
-        <v>US36</v>
-      </c>
-      <c r="C34" s="17" t="str">
-        <v>List recent deaths</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="17" t="str">
-        <v>US37</v>
-      </c>
-      <c r="C35" s="17" t="str">
-        <v>List recent survivors</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="17" t="str">
-        <v>US38</v>
-      </c>
-      <c r="C36" s="17" t="str">
-        <v>List upcoming birthdays</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="17" t="str">
-        <v>US39</v>
-      </c>
-      <c r="C37" s="17" t="str">
-        <v>List upcoming anniversaries</v>
-      </c>
+      <c r="A32" s="29"/>
+      <c r="B32" s="64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3573,7 +3650,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H10"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3703,7 +3780,7 @@
         <v>241</v>
       </c>
       <c r="L3" s="54" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M3" s="20" t="s">
         <v>231</v>
@@ -3712,7 +3789,7 @@
         <v>248</v>
       </c>
       <c r="O3" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3751,7 +3828,7 @@
         <v>242</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M4" s="20" t="s">
         <v>232</v>
@@ -3760,7 +3837,7 @@
         <v>249</v>
       </c>
       <c r="O4" s="57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3799,7 +3876,7 @@
         <v>243</v>
       </c>
       <c r="L5" s="52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M5" s="20" t="s">
         <v>233</v>
@@ -3808,7 +3885,7 @@
         <v>250</v>
       </c>
       <c r="O5" s="57" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3847,7 +3924,7 @@
         <v>244</v>
       </c>
       <c r="L6" s="52" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>234</v>
@@ -3856,7 +3933,7 @@
         <v>251</v>
       </c>
       <c r="O6" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3895,7 +3972,7 @@
         <v>240</v>
       </c>
       <c r="L7" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M7" s="21" t="s">
         <v>235</v>
@@ -3904,7 +3981,7 @@
         <v>248</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -3943,7 +4020,7 @@
         <v>245</v>
       </c>
       <c r="L8" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M8" s="20" t="s">
         <v>236</v>
@@ -3952,7 +4029,7 @@
         <v>248</v>
       </c>
       <c r="O8" s="57" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -3991,7 +4068,7 @@
         <v>246</v>
       </c>
       <c r="L9" s="52" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M9" s="20" t="s">
         <v>237</v>
@@ -4000,7 +4077,7 @@
         <v>252</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4039,7 +4116,7 @@
         <v>247</v>
       </c>
       <c r="L10" s="52" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M10" s="20" t="s">
         <v>238</v>
@@ -4048,7 +4125,7 @@
         <v>253</v>
       </c>
       <c r="O10" s="57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="14">
@@ -4161,10 +4238,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4186,7 +4263,7 @@
     <col min="15" max="15" width="10.1640625" style="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20" customHeight="1">
+    <row r="1" spans="1:16" ht="20" customHeight="1">
       <c r="A1" s="73" t="s">
         <v>3</v>
       </c>
@@ -4219,7 +4296,7 @@
       <c r="N1" s="74"/>
       <c r="O1" s="75"/>
     </row>
-    <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1">
+    <row r="2" spans="1:16" ht="20" customHeight="1" thickBot="1">
       <c r="A2" s="76"/>
       <c r="B2" s="78"/>
       <c r="C2" s="76"/>
@@ -4258,7 +4335,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14" thickTop="1">
+    <row r="3" spans="1:16" ht="14" thickTop="1">
       <c r="A3" s="13" t="s">
         <v>117</v>
       </c>
@@ -4284,28 +4361,28 @@
         <v>50</v>
       </c>
       <c r="I3" s="69" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K3" t="s">
         <v>266</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="M3" t="s">
         <v>267</v>
       </c>
-      <c r="L3" s="69" t="s">
-        <v>262</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>268</v>
       </c>
-      <c r="N3" t="s">
-        <v>269</v>
-      </c>
       <c r="O3" s="69" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="13" t="s">
         <v>121</v>
       </c>
@@ -4315,8 +4392,8 @@
       <c r="C4" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>208</v>
+      <c r="D4" t="s">
+        <v>239</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -4331,28 +4408,28 @@
         <v>30</v>
       </c>
       <c r="I4" s="69" t="s">
+        <v>276</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="J4" s="13" t="s">
-        <v>278</v>
-      </c>
       <c r="K4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L4" s="69" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O4" s="69" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="13" t="s">
         <v>123</v>
       </c>
@@ -4378,28 +4455,28 @@
         <v>120</v>
       </c>
       <c r="I5" s="69" t="s">
+        <v>269</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="K5" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="69" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="M5" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="O5" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="O5" s="69" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="13" t="s">
         <v>122</v>
       </c>
@@ -4409,8 +4486,8 @@
       <c r="C6" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>208</v>
+      <c r="D6" t="s">
+        <v>239</v>
       </c>
       <c r="E6">
         <v>60</v>
@@ -4425,28 +4502,28 @@
         <v>50</v>
       </c>
       <c r="I6" s="69" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L6" s="69" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="13" t="s">
         <v>128</v>
       </c>
@@ -4457,7 +4534,7 @@
         <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -4466,7 +4543,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" s="13" t="s">
         <v>129</v>
       </c>
@@ -4477,7 +4554,7 @@
         <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4486,7 +4563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" s="13" t="s">
         <v>126</v>
       </c>
@@ -4497,7 +4574,7 @@
         <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -4506,7 +4583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" s="13" t="s">
         <v>127</v>
       </c>
@@ -4517,7 +4594,7 @@
         <v>186</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>239</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -4525,6 +4602,299 @@
       <c r="F10">
         <v>20</v>
       </c>
+    </row>
+    <row r="13" spans="1:16" ht="14">
+      <c r="A13" s="64"/>
+      <c r="B13" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="81"/>
+    </row>
+    <row r="14" spans="1:16" ht="14">
+      <c r="A14" s="64"/>
+      <c r="B14" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="81"/>
+    </row>
+    <row r="15" spans="1:16" s="43" customFormat="1">
+      <c r="A15" s="39">
+        <v>1</v>
+      </c>
+      <c r="B15" s="87" t="s">
+        <v>290</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="47"/>
+    </row>
+    <row r="16" spans="1:16" s="43" customFormat="1">
+      <c r="A16" s="39">
+        <v>2</v>
+      </c>
+      <c r="B16" s="87" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="83"/>
+      <c r="K16" s="83"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="83"/>
+      <c r="N16" s="83"/>
+      <c r="O16" s="84"/>
+      <c r="P16" s="47"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="39"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="79"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="81"/>
+    </row>
+    <row r="18" spans="1:16" ht="14">
+      <c r="A18" s="64"/>
+      <c r="B18" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="81"/>
+    </row>
+    <row r="19" spans="1:16" s="43" customFormat="1" ht="17" customHeight="1">
+      <c r="A19" s="39">
+        <v>1</v>
+      </c>
+      <c r="B19" s="89" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="47"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="39"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="81"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="64"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="85"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="85"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="64"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="85"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="64"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="85"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="64"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="85"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="64"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="85"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="64"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="85"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="64"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="85"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="85"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="64"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4545,14 +4915,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
@@ -4631,7 +5002,130 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14" thickTop="1"/>
+    <row r="3" spans="1:15" ht="14" thickTop="1">
+      <c r="A3" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="J1:L1"/>
@@ -4650,10 +5144,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4738,6 +5232,11 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="14" thickTop="1"/>
+    <row r="19" spans="9:9">
+      <c r="I19" t="s">
+        <v>292</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="J1:L1"/>
@@ -4758,14 +5257,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B17"/>
+    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="29"/>
-    <col min="2" max="2" width="28.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" style="29" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="31" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="29"/>
   </cols>
@@ -4840,7 +5339,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:4" ht="34">
       <c r="A6" s="29" t="s">
         <v>116</v>
       </c>
@@ -4910,7 +5409,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34">
+    <row r="11" spans="1:4" ht="51">
       <c r="A11" s="29" t="s">
         <v>121</v>
       </c>
@@ -4934,6 +5433,9 @@
       <c r="C12" s="30" t="s">
         <v>41</v>
       </c>
+      <c r="D12" s="29" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="51">
       <c r="A13" s="29" t="s">
@@ -4959,6 +5461,9 @@
       <c r="C14" s="30" t="s">
         <v>171</v>
       </c>
+      <c r="D14" s="29" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="34">
       <c r="A15" s="29" t="s">
@@ -4970,6 +5475,9 @@
       <c r="C15" s="30" t="s">
         <v>42</v>
       </c>
+      <c r="D15" s="29" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="17">
       <c r="A16" s="29" t="s">
@@ -4981,6 +5489,9 @@
       <c r="C16" s="30" t="s">
         <v>43</v>
       </c>
+      <c r="D16" s="29" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="34">
       <c r="A17" s="29" t="s">
@@ -4992,6 +5503,9 @@
       <c r="C17" s="30" t="s">
         <v>44</v>
       </c>
+      <c r="D17" s="29" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="17">
       <c r="A18" s="29" t="s">
@@ -5031,6 +5545,9 @@
       <c r="C20" s="30" t="s">
         <v>46</v>
       </c>
+      <c r="D20" s="29" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="34">
       <c r="A21" s="29" t="s">
@@ -5042,6 +5559,9 @@
       <c r="C21" s="30" t="s">
         <v>47</v>
       </c>
+      <c r="D21" s="29" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="34">
       <c r="A22" s="29" t="s">
@@ -5053,6 +5573,9 @@
       <c r="C22" s="30" t="s">
         <v>87</v>
       </c>
+      <c r="D22" s="29" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="34">
       <c r="A23" s="29" t="s">
@@ -5064,6 +5587,9 @@
       <c r="C23" s="30" t="s">
         <v>88</v>
       </c>
+      <c r="D23" s="29" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="34">
       <c r="A24" s="29" t="s">
@@ -5075,6 +5601,9 @@
       <c r="C24" s="30" t="s">
         <v>48</v>
       </c>
+      <c r="D24" s="29" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="51">
       <c r="A25" s="29" t="s">
@@ -5086,6 +5615,9 @@
       <c r="C25" s="30" t="s">
         <v>49</v>
       </c>
+      <c r="D25" s="29" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="34">
       <c r="A26" s="29" t="s">
@@ -5109,7 +5641,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17">
+    <row r="28" spans="1:4" ht="34">
       <c r="A28" s="29" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Sprint 3 update by yzhou
</commit_message>
<xml_diff>
--- a/docs/TeamHogwartsReport.xlsx
+++ b/docs/TeamHogwartsReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huying/GitHub/ssw555tmHogwarts2020Spring/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeyiszy/PycharmProjects/ssw555tmHogwarts2020Spring/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8BE332-73CE-614C-B6E4-E9FD2EC64CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C23CC-E7EB-AC48-86EB-A78604628D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="326">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1062,6 +1062,46 @@
   </si>
   <si>
     <t>us15.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us13.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us14.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us13_sibling_spacing</t>
+  </si>
+  <si>
+    <t>us14_multiple_births</t>
+  </si>
+  <si>
+    <t>6-30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6-24</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us13_test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us14_test</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_sibling_spacing</t>
+  </si>
+  <si>
+    <t>test_multiple_births</t>
+  </si>
+  <si>
+    <t>10-17</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1070,8 +1110,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="m/d"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1324,18 +1364,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1367,7 +1407,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1409,7 +1449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1451,24 +1491,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1516,74 +1556,81 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="30" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1601,7 +1648,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1748,7 +1795,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5137,8 +5184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -5241,6 +5288,33 @@
       <c r="F3" s="13">
         <v>50</v>
       </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3" s="93">
+        <v>180</v>
+      </c>
+      <c r="I3" s="94">
+        <v>42463</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="K3" t="s">
+        <v>317</v>
+      </c>
+      <c r="L3" s="95" t="s">
+        <v>320</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="N3" t="s">
+        <v>323</v>
+      </c>
+      <c r="O3" s="95" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="29" t="s">
@@ -5260,6 +5334,33 @@
       </c>
       <c r="F4" s="13">
         <v>60</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="I4" s="94">
+        <v>42463</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="K4" t="s">
+        <v>318</v>
+      </c>
+      <c r="L4" s="95" t="s">
+        <v>319</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="N4" t="s">
+        <v>324</v>
+      </c>
+      <c r="O4" s="95" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -5595,7 +5696,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34">
+    <row r="6" spans="1:4" ht="17">
       <c r="A6" s="29" t="s">
         <v>114</v>
       </c>
@@ -5665,7 +5766,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51">
+    <row r="11" spans="1:4" ht="34">
       <c r="A11" s="29" t="s">
         <v>119</v>
       </c>
@@ -5897,7 +5998,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34">
+    <row r="28" spans="1:4" ht="17">
       <c r="A28" s="29" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
update team report add comments for us23 and us 24
</commit_message>
<xml_diff>
--- a/docs/TeamHogwartsReport.xlsx
+++ b/docs/TeamHogwartsReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeyiszy/PycharmProjects/ssw555tmHogwarts2020Spring/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huying/GitHub/ssw555tmHogwarts2020Spring/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45C23CC-E7EB-AC48-86EB-A78604628D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD76255A-A26A-F742-A9DA-6A1C1C4831F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="335">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -713,9 +713,6 @@
     <t>To do</t>
   </si>
   <si>
-    <t>*Status: To do, coding, testing, done</t>
-  </si>
-  <si>
     <t>wuhuwuhuhu</t>
   </si>
   <si>
@@ -1103,6 +1100,36 @@
   <si>
     <t>10-17</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>us23.py</t>
+  </si>
+  <si>
+    <t>us23_unique_name_birth_date</t>
+  </si>
+  <si>
+    <t>us24.py</t>
+  </si>
+  <si>
+    <t>us24_unique_families_by_spouses</t>
+  </si>
+  <si>
+    <t>us23_test</t>
+  </si>
+  <si>
+    <t>us24_test</t>
+  </si>
+  <si>
+    <t>test_us23_unique_name_birth_date</t>
+  </si>
+  <si>
+    <t>test_us24_unique_families_by_spouses</t>
+  </si>
+  <si>
+    <t>*Status: To do, doing, done</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1137,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1364,18 +1391,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1407,7 +1434,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1449,7 +1476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1491,24 +1518,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1529,6 +1556,13 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1556,81 +1590,80 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="30" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="65" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1648,7 +1681,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1795,7 +1828,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2813,7 +2846,7 @@
         <v>194</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2830,7 +2863,7 @@
         <v>195</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2860,31 +2893,31 @@
     </row>
     <row r="9" spans="1:7">
       <c r="D9" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>209</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28" customHeight="1">
       <c r="D10" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E10" s="87" t="s">
         <v>211</v>
       </c>
-      <c r="E10" s="84" t="s">
-        <v>212</v>
-      </c>
-      <c r="F10" s="85"/>
-      <c r="G10" s="85"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
     </row>
     <row r="11" spans="1:7" ht="66" customHeight="1">
       <c r="D11" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="89" t="s">
         <v>213</v>
       </c>
-      <c r="E11" s="86" t="s">
-        <v>214</v>
-      </c>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
@@ -2911,7 +2944,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -2940,7 +2973,7 @@
         <v>28</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>206</v>
+        <v>334</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
@@ -3269,7 +3302,7 @@
       </c>
       <c r="E18" s="29" t="str">
         <f>Sprint3!D3</f>
-        <v>To do</v>
+        <v>done</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3290,7 +3323,7 @@
       </c>
       <c r="E19" s="29" t="str">
         <f>Sprint3!D4</f>
-        <v>To do</v>
+        <v>done</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3395,7 +3428,7 @@
       </c>
       <c r="E24" s="29" t="str">
         <f>Sprint3!D9</f>
-        <v>To do</v>
+        <v>done</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3416,7 +3449,7 @@
       </c>
       <c r="E25" s="29" t="str">
         <f>Sprint3!D10</f>
-        <v>To do</v>
+        <v>done</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3659,7 +3692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -3684,7 +3717,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>23</v>
@@ -3802,7 +3835,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:H4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -3825,43 +3858,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="16" customFormat="1" ht="28" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="87" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="90" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="87" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="92"/>
     </row>
     <row r="2" spans="1:16" s="16" customFormat="1" ht="28" customHeight="1" thickBot="1">
-      <c r="A2" s="90"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -3907,7 +3940,7 @@
         <v>198</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E3" s="17">
         <v>10</v>
@@ -3926,22 +3959,22 @@
         <v>42423</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L3" s="54" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O3" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -3955,7 +3988,7 @@
         <v>198</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E4" s="17">
         <v>10</v>
@@ -3974,22 +4007,22 @@
         <v>42423</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O4" s="57" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4003,7 +4036,7 @@
         <v>200</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5" s="17">
         <v>15</v>
@@ -4022,22 +4055,22 @@
         <v>42425</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L5" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O5" s="57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4051,7 +4084,7 @@
         <v>200</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="17">
         <v>15</v>
@@ -4070,22 +4103,22 @@
         <v>42425</v>
       </c>
       <c r="J6" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L6" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O6" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4099,7 +4132,7 @@
         <v>182</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E7" s="17">
         <v>15</v>
@@ -4118,22 +4151,22 @@
         <v>42417</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L7" s="52" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O7" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4147,7 +4180,7 @@
         <v>182</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E8" s="17">
         <v>10</v>
@@ -4166,22 +4199,22 @@
         <v>42417</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L8" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="O8" s="57" t="s">
         <v>254</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>233</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="O8" s="57" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -4195,7 +4228,7 @@
         <v>183</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E9" s="17">
         <v>6</v>
@@ -4214,22 +4247,22 @@
         <v>42425</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L9" s="52" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O9" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4243,7 +4276,7 @@
         <v>183</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10" s="17">
         <v>6</v>
@@ -4262,22 +4295,22 @@
         <v>42425</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L10" s="52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O10" s="57" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -4298,7 +4331,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="41"/>
@@ -4318,7 +4351,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="41"/>
@@ -4338,7 +4371,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="14">
@@ -4351,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="41"/>
@@ -4371,7 +4404,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4419,43 +4452,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="87" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="90" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="87" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="92"/>
     </row>
     <row r="2" spans="1:16" ht="20" customHeight="1" thickBot="1">
-      <c r="A2" s="90"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -4501,7 +4534,7 @@
         <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -4516,25 +4549,25 @@
         <v>50</v>
       </c>
       <c r="I3" s="69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J3" t="s">
+        <v>261</v>
+      </c>
+      <c r="K3" t="s">
         <v>262</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="69" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" t="s">
         <v>263</v>
       </c>
-      <c r="L3" s="69" t="s">
-        <v>258</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>264</v>
       </c>
-      <c r="N3" t="s">
-        <v>265</v>
-      </c>
       <c r="O3" s="69" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -4548,7 +4581,7 @@
         <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -4563,25 +4596,25 @@
         <v>30</v>
       </c>
       <c r="I4" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="J4" s="13" t="s">
-        <v>273</v>
-      </c>
       <c r="K4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L4" s="69" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O4" s="69" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4595,7 +4628,7 @@
         <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E5">
         <v>60</v>
@@ -4610,25 +4643,25 @@
         <v>120</v>
       </c>
       <c r="I5" s="69" t="s">
+        <v>265</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="K5" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="L5" s="69" t="s">
         <v>268</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="M5" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="O5" s="69" t="s">
         <v>270</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="O5" s="69" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4642,7 +4675,7 @@
         <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6">
         <v>60</v>
@@ -4657,25 +4690,25 @@
         <v>50</v>
       </c>
       <c r="I6" s="69" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L6" s="69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4689,7 +4722,7 @@
         <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -4704,25 +4737,25 @@
         <v>40</v>
       </c>
       <c r="I7" s="68" t="s">
+        <v>288</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>290</v>
-      </c>
       <c r="K7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L7" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="O7" s="69" t="s">
         <v>260</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="O7" s="69" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4736,7 +4769,7 @@
         <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -4751,25 +4784,25 @@
         <v>80</v>
       </c>
       <c r="I8" s="68" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L8" s="69" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M8" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O8" s="69" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -4783,7 +4816,7 @@
         <v>183</v>
       </c>
       <c r="D9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -4798,25 +4831,25 @@
         <v>8</v>
       </c>
       <c r="I9" s="69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L9" s="69" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M9" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O9" s="69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -4830,7 +4863,7 @@
         <v>183</v>
       </c>
       <c r="D10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10">
         <v>15</v>
@@ -4845,25 +4878,25 @@
         <v>20</v>
       </c>
       <c r="I10" s="69" t="s">
+        <v>297</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="J10" s="15" t="s">
-        <v>299</v>
-      </c>
       <c r="K10" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L10" s="69" t="s">
+        <v>305</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="N10" t="s">
         <v>306</v>
       </c>
-      <c r="M10" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="N10" t="s">
-        <v>307</v>
-      </c>
       <c r="O10" s="69" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -4913,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="78" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -4935,7 +4968,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -4993,7 +5026,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="80" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -5185,7 +5218,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -5193,48 +5226,48 @@
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="68" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="87" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="90" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="87" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="92"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1">
-      <c r="A2" s="90"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -5256,7 +5289,7 @@
       <c r="K2" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="50" t="s">
         <v>176</v>
       </c>
       <c r="M2" s="22" t="s">
@@ -5280,7 +5313,7 @@
         <v>179</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>205</v>
+        <v>325</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -5291,29 +5324,29 @@
       <c r="G3">
         <v>13</v>
       </c>
-      <c r="H3" s="93">
+      <c r="H3" s="84">
         <v>180</v>
       </c>
-      <c r="I3" s="94">
+      <c r="I3" s="85">
         <v>42463</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K3" t="s">
-        <v>317</v>
-      </c>
-      <c r="L3" s="95" t="s">
+        <v>316</v>
+      </c>
+      <c r="L3" s="86" t="s">
+        <v>319</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="M3" s="13" t="s">
-        <v>321</v>
-      </c>
       <c r="N3" t="s">
-        <v>323</v>
-      </c>
-      <c r="O3" s="95" t="s">
-        <v>325</v>
+        <v>322</v>
+      </c>
+      <c r="O3" s="86" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -5327,7 +5360,7 @@
         <v>179</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>205</v>
+        <v>325</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -5341,26 +5374,26 @@
       <c r="H4">
         <v>40</v>
       </c>
-      <c r="I4" s="94">
+      <c r="I4" s="85">
         <v>42463</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K4" t="s">
+        <v>317</v>
+      </c>
+      <c r="L4" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="L4" s="95" t="s">
-        <v>319</v>
-      </c>
       <c r="M4" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N4" t="s">
+        <v>323</v>
+      </c>
+      <c r="O4" s="86" t="s">
         <v>324</v>
-      </c>
-      <c r="O4" s="95" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -5454,13 +5487,40 @@
         <v>188</v>
       </c>
       <c r="D9" s="82" t="s">
-        <v>205</v>
+        <v>325</v>
       </c>
       <c r="E9">
         <v>30</v>
       </c>
       <c r="F9">
         <v>50</v>
+      </c>
+      <c r="G9">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>120</v>
+      </c>
+      <c r="I9" s="85">
+        <v>42463</v>
+      </c>
+      <c r="J9" t="s">
+        <v>326</v>
+      </c>
+      <c r="K9" t="s">
+        <v>327</v>
+      </c>
+      <c r="L9" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="O9" s="96" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -5474,13 +5534,40 @@
         <v>188</v>
       </c>
       <c r="D10" s="82" t="s">
-        <v>205</v>
+        <v>325</v>
       </c>
       <c r="E10">
         <v>30</v>
       </c>
       <c r="F10">
         <v>50</v>
+      </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10" s="85">
+        <v>42463</v>
+      </c>
+      <c r="J10" t="s">
+        <v>328</v>
+      </c>
+      <c r="K10" t="s">
+        <v>329</v>
+      </c>
+      <c r="L10" s="86" t="s">
+        <v>253</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="O10" s="97" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -5517,43 +5604,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="87" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="90" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="87" t="s">
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="87" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="90" t="s">
         <v>204</v>
       </c>
-      <c r="N1" s="88"/>
-      <c r="O1" s="89"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="92"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1">
-      <c r="A2" s="90"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -5591,7 +5678,7 @@
     <row r="3" spans="1:15" ht="14" thickTop="1"/>
     <row r="19" spans="9:9">
       <c r="I19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -5696,7 +5783,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:4" ht="34">
       <c r="A6" s="29" t="s">
         <v>114</v>
       </c>
@@ -5766,7 +5853,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34">
+    <row r="11" spans="1:4" ht="51">
       <c r="A11" s="29" t="s">
         <v>119</v>
       </c>
@@ -5774,7 +5861,7 @@
         <v>74</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>179</v>
@@ -5844,7 +5931,7 @@
         <v>79</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>183</v>
@@ -5858,7 +5945,7 @@
         <v>80</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>183</v>
@@ -5998,7 +6085,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17">
+    <row r="28" spans="1:4" ht="34">
       <c r="A28" s="29" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
Add US29_TEST, US30_TEST to travis command
</commit_message>
<xml_diff>
--- a/docs/TeamHogwartsReport.xlsx
+++ b/docs/TeamHogwartsReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huying/GitHub/ssw555tmHogwarts2020Spring/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeyiszy/PycharmProjects/ssw555tmHogwarts2020Spring/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E91214E-0A05-C248-ACA2-B21B78ADDD7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732BFD71-54E7-4941-A853-450C31AA76EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="560" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="540" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="402">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1337,6 +1337,52 @@
   </si>
   <si>
     <t>1-28</t>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>15</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us31.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us32.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us31_list_living_single</t>
+  </si>
+  <si>
+    <t>us32_list_mutiple_births</t>
+  </si>
+  <si>
+    <t>6-13</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us31_test.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>us32_test.py</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_list_living_single</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_list_mutiple_births</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1344,8 +1390,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="m/d"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1612,16 +1658,16 @@
   </cellStyleXfs>
   <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1653,7 +1699,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1695,7 +1741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1737,24 +1783,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1793,12 +1839,32 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1831,94 +1897,74 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="66">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1936,7 +1982,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2083,7 +2129,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3169,21 +3215,21 @@
       <c r="D10" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="E10" s="96" t="s">
+      <c r="E10" s="104" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
     </row>
     <row r="11" spans="1:7" ht="66" customHeight="1">
       <c r="D11" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="98" t="s">
+      <c r="E11" s="106" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C4">
@@ -4296,43 +4342,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="16" customFormat="1" ht="28" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="100"/>
-      <c r="G1" s="99" t="s">
+      <c r="F1" s="108"/>
+      <c r="G1" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="99" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="99" t="s">
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="101"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="109"/>
     </row>
     <row r="2" spans="1:16" s="16" customFormat="1" ht="28" customHeight="1" thickBot="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="104"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -4890,43 +4936,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="100"/>
-      <c r="G1" s="99" t="s">
+      <c r="F1" s="108"/>
+      <c r="G1" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="99" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="99" t="s">
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="101"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="109"/>
     </row>
     <row r="2" spans="1:16" ht="20" customHeight="1" thickBot="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="104"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -5655,7 +5701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -5669,43 +5715,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="100"/>
-      <c r="G1" s="99" t="s">
+      <c r="F1" s="108"/>
+      <c r="G1" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="99" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="99" t="s">
+      <c r="K1" s="108"/>
+      <c r="L1" s="108"/>
+      <c r="M1" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="101"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="109"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="104"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
       <c r="E2" s="22" t="s">
         <v>13</v>
       </c>
@@ -6146,13 +6192,13 @@
     </row>
     <row r="17" spans="1:6" ht="26" customHeight="1">
       <c r="A17" s="39"/>
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="113" t="s">
         <v>364</v>
       </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
     </row>
     <row r="18" spans="1:6" ht="14">
       <c r="A18" s="64"/>
@@ -6191,7 +6237,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -6205,43 +6251,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="99" t="s">
+      <c r="D1" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="101"/>
-      <c r="G1" s="99" t="s">
+      <c r="F1" s="109"/>
+      <c r="G1" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="100"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="99" t="s">
+      <c r="H1" s="108"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="K1" s="100"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="99" t="s">
+      <c r="K1" s="108"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="100"/>
-      <c r="O1" s="101"/>
+      <c r="N1" s="108"/>
+      <c r="O1" s="109"/>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1" thickBot="1">
-      <c r="A2" s="102"/>
-      <c r="B2" s="104"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
       <c r="E2" s="89" t="s">
         <v>13</v>
       </c>
@@ -6301,22 +6347,22 @@
       <c r="H3" s="39">
         <v>15</v>
       </c>
-      <c r="I3" s="106">
+      <c r="I3" s="96">
         <v>42470</v>
       </c>
-      <c r="J3" s="112" t="s">
+      <c r="J3" s="102" t="s">
         <v>379</v>
       </c>
-      <c r="K3" s="108" t="s">
+      <c r="K3" s="98" t="s">
         <v>381</v>
       </c>
       <c r="L3" s="95" t="s">
         <v>383</v>
       </c>
-      <c r="M3" s="111" t="s">
+      <c r="M3" s="101" t="s">
         <v>385</v>
       </c>
-      <c r="N3" s="113" t="s">
+      <c r="N3" s="103" t="s">
         <v>387</v>
       </c>
       <c r="O3" s="95" t="s">
@@ -6348,22 +6394,22 @@
       <c r="H4" s="39">
         <v>15</v>
       </c>
-      <c r="I4" s="106">
+      <c r="I4" s="96">
         <v>42470</v>
       </c>
-      <c r="J4" s="112" t="s">
+      <c r="J4" s="102" t="s">
         <v>380</v>
       </c>
-      <c r="K4" s="108" t="s">
+      <c r="K4" s="98" t="s">
         <v>382</v>
       </c>
       <c r="L4" s="95" t="s">
         <v>384</v>
       </c>
-      <c r="M4" s="111" t="s">
+      <c r="M4" s="101" t="s">
         <v>386</v>
       </c>
-      <c r="N4" s="113" t="s">
+      <c r="N4" s="103" t="s">
         <v>388</v>
       </c>
       <c r="O4" s="95" t="s">
@@ -6389,15 +6435,33 @@
       <c r="F5" s="29">
         <v>120</v>
       </c>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="109"/>
-      <c r="N5" s="109"/>
-      <c r="O5" s="95"/>
+      <c r="G5" s="99" t="s">
+        <v>390</v>
+      </c>
+      <c r="H5" s="99" t="s">
+        <v>392</v>
+      </c>
+      <c r="I5" s="97">
+        <v>42477</v>
+      </c>
+      <c r="J5" s="99" t="s">
+        <v>393</v>
+      </c>
+      <c r="K5" s="100" t="s">
+        <v>395</v>
+      </c>
+      <c r="L5" s="95" t="s">
+        <v>397</v>
+      </c>
+      <c r="M5" s="100" t="s">
+        <v>398</v>
+      </c>
+      <c r="N5" s="99" t="s">
+        <v>400</v>
+      </c>
+      <c r="O5" s="95" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="29" t="s">
@@ -6418,15 +6482,33 @@
       <c r="F6" s="29">
         <v>50</v>
       </c>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="109"/>
-      <c r="N6" s="109"/>
-      <c r="O6" s="95"/>
+      <c r="G6" s="99" t="s">
+        <v>390</v>
+      </c>
+      <c r="H6" s="99" t="s">
+        <v>391</v>
+      </c>
+      <c r="I6" s="97">
+        <v>42477</v>
+      </c>
+      <c r="J6" s="99" t="s">
+        <v>394</v>
+      </c>
+      <c r="K6" s="100" t="s">
+        <v>396</v>
+      </c>
+      <c r="L6" s="95" t="s">
+        <v>397</v>
+      </c>
+      <c r="M6" s="100" t="s">
+        <v>399</v>
+      </c>
+      <c r="N6" s="99" t="s">
+        <v>401</v>
+      </c>
+      <c r="O6" s="95" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="29" t="s">
@@ -6447,28 +6529,28 @@
       <c r="F7" s="29">
         <v>30</v>
       </c>
-      <c r="G7" s="109">
+      <c r="G7" s="99">
         <v>9</v>
       </c>
-      <c r="H7" s="109">
+      <c r="H7" s="99">
         <v>40</v>
       </c>
-      <c r="I7" s="107">
+      <c r="I7" s="97">
         <v>42470</v>
       </c>
-      <c r="J7" s="109" t="s">
+      <c r="J7" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="K7" s="110" t="s">
+      <c r="K7" s="100" t="s">
         <v>371</v>
       </c>
       <c r="L7" s="95" t="s">
         <v>373</v>
       </c>
-      <c r="M7" s="111" t="s">
+      <c r="M7" s="101" t="s">
         <v>374</v>
       </c>
-      <c r="N7" s="109" t="s">
+      <c r="N7" s="99" t="s">
         <v>376</v>
       </c>
       <c r="O7" s="95" t="s">
@@ -6494,28 +6576,28 @@
       <c r="F8" s="29">
         <v>30</v>
       </c>
-      <c r="G8" s="109">
+      <c r="G8" s="99">
         <v>9</v>
       </c>
-      <c r="H8" s="109">
+      <c r="H8" s="99">
         <v>20</v>
       </c>
-      <c r="I8" s="107">
+      <c r="I8" s="97">
         <v>42470</v>
       </c>
-      <c r="J8" s="109" t="s">
+      <c r="J8" s="99" t="s">
         <v>370</v>
       </c>
-      <c r="K8" s="110" t="s">
+      <c r="K8" s="100" t="s">
         <v>372</v>
       </c>
       <c r="L8" s="95" t="s">
         <v>373</v>
       </c>
-      <c r="M8" s="111" t="s">
+      <c r="M8" s="101" t="s">
         <v>375</v>
       </c>
-      <c r="N8" s="109" t="s">
+      <c r="N8" s="99" t="s">
         <v>377</v>
       </c>
       <c r="O8" s="95" t="s">
@@ -6541,14 +6623,14 @@
       <c r="F9" s="29">
         <v>30</v>
       </c>
-      <c r="G9" s="109"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="107"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="109"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
       <c r="L9" s="95"/>
-      <c r="M9" s="109"/>
-      <c r="N9" s="109"/>
+      <c r="M9" s="99"/>
+      <c r="N9" s="99"/>
       <c r="O9" s="95"/>
     </row>
     <row r="10" spans="1:15">
@@ -6572,7 +6654,7 @@
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="64"/>
-      <c r="I10" s="106"/>
+      <c r="I10" s="96"/>
       <c r="J10" s="17"/>
       <c r="K10" s="64"/>
       <c r="L10" s="94"/>
@@ -6606,8 +6688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
@@ -6688,7 +6770,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34">
+    <row r="6" spans="1:4" ht="17">
       <c r="A6" s="29" t="s">
         <v>89</v>
       </c>
@@ -6758,7 +6840,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="51">
+    <row r="11" spans="1:4" ht="34">
       <c r="A11" s="29" t="s">
         <v>94</v>
       </c>
@@ -6990,7 +7072,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="34">
+    <row r="28" spans="1:4" ht="17">
       <c r="A28" s="29" t="s">
         <v>111</v>
       </c>

</xml_diff>